<commit_message>
Updated scripts to fit README.md
</commit_message>
<xml_diff>
--- a/data/normalized_library_data.xlsx
+++ b/data/normalized_library_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Repositories\dbsigmarizz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Repositories\dbsigmarizz\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1869FB3F-BEAA-4CD2-BD25-0357FB2163FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D32A044-13E2-4B27-9D36-E9C359BFFAB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="12456" xr2:uid="{21EFF67A-8CF7-4130-836C-CA8B707EBEF1}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="339">
   <si>
     <t>ID</t>
   </si>
@@ -784,9 +784,6 @@
     <t>U-c351e4ee-8eed-11ef-834d-08bfb82c14c5</t>
   </si>
   <si>
-    <t>ReservationDate</t>
-  </si>
-  <si>
     <t>Username</t>
   </si>
   <si>
@@ -1037,12 +1034,6 @@
   </si>
   <si>
     <t>User</t>
-  </si>
-  <si>
-    <t>Loan</t>
-  </si>
-  <si>
-    <t>Reservation</t>
   </si>
   <si>
     <t>Return (History)</t>
@@ -1550,15 +1541,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -1938,7 +1927,7 @@
   <dimension ref="A1:X197"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1968,76 +1957,84 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B1" t="s">
+        <v>335</v>
+      </c>
+      <c r="E1" t="s">
         <v>336</v>
       </c>
-      <c r="B1" t="s">
-        <v>336</v>
-      </c>
-      <c r="E1" s="5" t="s">
+      <c r="M1" t="s">
+        <v>338</v>
+      </c>
+      <c r="S1" t="s">
         <v>337</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="S1" t="s">
-        <v>338</v>
-      </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="M2" t="s">
-        <v>340</v>
-      </c>
-      <c r="R2" s="5"/>
-      <c r="S2" s="8" t="s">
+      <c r="M2" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="S2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="T2" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="U2" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="U2" s="8" t="s">
+      <c r="V2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="V2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="W2" s="8" t="s">
+      <c r="X2" s="6" t="s">
         <v>257</v>
-      </c>
-      <c r="X2" s="8" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
@@ -2071,33 +2068,39 @@
       <c r="K3" s="3">
         <v>10</v>
       </c>
-      <c r="M3" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>254</v>
-      </c>
-      <c r="R3" s="7"/>
+      <c r="M3" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="P3" s="5">
+        <v>45391</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>45525</v>
+      </c>
+      <c r="R3" s="2"/>
       <c r="S3" s="3" t="s">
         <v>235</v>
       </c>
       <c r="T3" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="U3" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="W3" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="X3" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
@@ -2131,24 +2134,39 @@
       <c r="K4" s="3">
         <v>1</v>
       </c>
-      <c r="R4" s="7"/>
+      <c r="M4" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="P4" s="5">
+        <v>45336</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>45509</v>
+      </c>
+      <c r="R4" s="2"/>
       <c r="S4" s="3" t="s">
         <v>236</v>
       </c>
       <c r="T4" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="V4" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="U4" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="V4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="X4" s="3" t="s">
         <v>266</v>
-      </c>
-      <c r="X4" s="3" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
@@ -2182,27 +2200,39 @@
       <c r="K5" s="3">
         <v>3</v>
       </c>
-      <c r="M5" t="s">
-        <v>339</v>
-      </c>
-      <c r="R5" s="7"/>
+      <c r="M5" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="P5" s="5">
+        <v>45413</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>45504</v>
+      </c>
+      <c r="R5" s="2"/>
       <c r="S5" s="3" t="s">
         <v>237</v>
       </c>
       <c r="T5" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="V5" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="U5" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="V5" s="3" t="s">
+      <c r="W5" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="W5" s="3" t="s">
+      <c r="X5" s="3" t="s">
         <v>270</v>
-      </c>
-      <c r="X5" s="3" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
@@ -2236,33 +2266,39 @@
       <c r="K6" s="3">
         <v>11</v>
       </c>
-      <c r="M6" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="N6" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="O6" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="R6" s="7"/>
+      <c r="M6" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="P6" s="5">
+        <v>45397</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>45535</v>
+      </c>
+      <c r="R6" s="2"/>
       <c r="S6" s="3" t="s">
         <v>238</v>
       </c>
       <c r="T6" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="V6" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="U6" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="V6" s="3" t="s">
+      <c r="W6" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="W6" s="3" t="s">
+      <c r="X6" s="3" t="s">
         <v>274</v>
-      </c>
-      <c r="X6" s="3" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.3">
@@ -2296,24 +2332,39 @@
       <c r="K7" s="3">
         <v>1</v>
       </c>
-      <c r="R7" s="7"/>
+      <c r="M7" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="P7" s="5">
+        <v>45527</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>45543</v>
+      </c>
+      <c r="R7" s="2"/>
       <c r="S7" s="3" t="s">
         <v>239</v>
       </c>
       <c r="T7" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="V7" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="U7" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="V7" s="3" t="s">
+      <c r="W7" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="W7" s="3" t="s">
+      <c r="X7" s="3" t="s">
         <v>278</v>
-      </c>
-      <c r="X7" s="3" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.3">
@@ -2347,27 +2398,39 @@
       <c r="K8" s="3">
         <v>15</v>
       </c>
-      <c r="M8" t="s">
-        <v>341</v>
-      </c>
-      <c r="R8" s="7"/>
+      <c r="M8" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="P8" s="5">
+        <v>45406</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>45484</v>
+      </c>
+      <c r="R8" s="2"/>
       <c r="S8" s="3" t="s">
         <v>240</v>
       </c>
       <c r="T8" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="V8" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="U8" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="V8" s="3" t="s">
+      <c r="W8" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="W8" s="3" t="s">
+      <c r="X8" s="3" t="s">
         <v>282</v>
-      </c>
-      <c r="X8" s="3" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.3">
@@ -2401,39 +2464,39 @@
       <c r="K9" s="3">
         <v>12</v>
       </c>
-      <c r="M9" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="N9" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="O9" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="P9" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="Q9" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="R9" s="7"/>
+      <c r="M9" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="P9" s="5">
+        <v>45549</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>45556</v>
+      </c>
+      <c r="R9" s="2"/>
       <c r="S9" s="3" t="s">
         <v>241</v>
       </c>
       <c r="T9" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="U9" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="V9" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="U9" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="V9" s="3" t="s">
+      <c r="W9" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="W9" s="3" t="s">
+      <c r="X9" s="3" t="s">
         <v>286</v>
-      </c>
-      <c r="X9" s="3" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.3">
@@ -2468,38 +2531,38 @@
         <v>2</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>97</v>
+        <v>122</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="O10" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P10" s="6">
-        <v>45391</v>
-      </c>
-      <c r="Q10" s="6">
-        <v>45525</v>
-      </c>
-      <c r="R10" s="7"/>
+      <c r="P10" s="5">
+        <v>45389</v>
+      </c>
+      <c r="Q10" s="5">
+        <v>45515</v>
+      </c>
+      <c r="R10" s="2"/>
       <c r="S10" s="3" t="s">
         <v>242</v>
       </c>
       <c r="T10" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="U10" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="V10" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="U10" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="V10" s="3" t="s">
+      <c r="W10" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="W10" s="3" t="s">
+      <c r="X10" s="3" t="s">
         <v>290</v>
-      </c>
-      <c r="X10" s="3" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.3">
@@ -2534,38 +2597,38 @@
         <v>15</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="O11" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P11" s="6">
-        <v>45336</v>
-      </c>
-      <c r="Q11" s="6">
-        <v>45509</v>
-      </c>
-      <c r="R11" s="7"/>
+      <c r="P11" s="5">
+        <v>45372</v>
+      </c>
+      <c r="Q11" s="5">
+        <v>45383</v>
+      </c>
+      <c r="R11" s="2"/>
       <c r="S11" s="3" t="s">
         <v>243</v>
       </c>
       <c r="T11" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="U11" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="V11" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="U11" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="V11" s="3" t="s">
+      <c r="W11" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="W11" s="3" t="s">
+      <c r="X11" s="3" t="s">
         <v>294</v>
-      </c>
-      <c r="X11" s="3" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.3">
@@ -2600,38 +2663,38 @@
         <v>11</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="O12" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P12" s="6">
-        <v>45413</v>
-      </c>
-      <c r="Q12" s="6">
-        <v>45504</v>
-      </c>
-      <c r="R12" s="7"/>
+      <c r="P12" s="5">
+        <v>45310</v>
+      </c>
+      <c r="Q12" s="5">
+        <v>45351</v>
+      </c>
+      <c r="R12" s="2"/>
       <c r="S12" s="3" t="s">
         <v>244</v>
       </c>
       <c r="T12" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="U12" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="V12" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="U12" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="V12" s="3" t="s">
+      <c r="W12" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="W12" s="3" t="s">
+      <c r="X12" s="3" t="s">
         <v>298</v>
-      </c>
-      <c r="X12" s="3" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.3">
@@ -2666,38 +2729,38 @@
         <v>9</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>110</v>
+        <v>131</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="O13" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P13" s="6">
-        <v>45397</v>
-      </c>
-      <c r="Q13" s="6">
-        <v>45535</v>
-      </c>
-      <c r="R13" s="7"/>
+      <c r="P13" s="5">
+        <v>45295</v>
+      </c>
+      <c r="Q13" s="5">
+        <v>45358</v>
+      </c>
+      <c r="R13" s="2"/>
       <c r="S13" s="3" t="s">
         <v>250</v>
       </c>
       <c r="T13" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="U13" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="V13" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="U13" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="V13" s="3" t="s">
+      <c r="W13" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="W13" s="3" t="s">
+      <c r="X13" s="3" t="s">
         <v>302</v>
-      </c>
-      <c r="X13" s="3" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.3">
@@ -2732,38 +2795,38 @@
         <v>12</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="O14" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P14" s="6">
-        <v>45527</v>
-      </c>
-      <c r="Q14" s="6">
-        <v>45543</v>
-      </c>
-      <c r="R14" s="7"/>
+      <c r="P14" s="5">
+        <v>45306</v>
+      </c>
+      <c r="Q14" s="5">
+        <v>45460</v>
+      </c>
+      <c r="R14" s="2"/>
       <c r="S14" s="3" t="s">
         <v>245</v>
       </c>
       <c r="T14" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="U14" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="V14" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="U14" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="V14" s="3" t="s">
+      <c r="W14" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="W14" s="3" t="s">
+      <c r="X14" s="3" t="s">
         <v>306</v>
-      </c>
-      <c r="X14" s="3" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.3">
@@ -2798,38 +2861,38 @@
         <v>3</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="O15" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P15" s="6">
-        <v>45406</v>
-      </c>
-      <c r="Q15" s="6">
-        <v>45484</v>
-      </c>
-      <c r="R15" s="7"/>
+      <c r="P15" s="5">
+        <v>45539</v>
+      </c>
+      <c r="Q15" s="5">
+        <v>45552</v>
+      </c>
+      <c r="R15" s="2"/>
       <c r="S15" s="3" t="s">
         <v>246</v>
       </c>
       <c r="T15" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="U15" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="V15" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="U15" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="V15" s="3" t="s">
+      <c r="W15" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="W15" s="3" t="s">
+      <c r="X15" s="3" t="s">
         <v>310</v>
-      </c>
-      <c r="X15" s="3" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.3">
@@ -2864,38 +2927,38 @@
         <v>7</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="O16" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P16" s="6">
-        <v>45549</v>
-      </c>
-      <c r="Q16" s="6">
-        <v>45556</v>
-      </c>
-      <c r="R16" s="7"/>
+      <c r="P16" s="5">
+        <v>45480</v>
+      </c>
+      <c r="Q16" s="5">
+        <v>45515</v>
+      </c>
+      <c r="R16" s="2"/>
       <c r="S16" s="3" t="s">
         <v>247</v>
       </c>
       <c r="T16" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="U16" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="V16" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="U16" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="V16" s="3" t="s">
+      <c r="W16" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="W16" s="3" t="s">
+      <c r="X16" s="3" t="s">
         <v>314</v>
-      </c>
-      <c r="X16" s="3" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.3">
@@ -2930,38 +2993,38 @@
         <v>14</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>122</v>
+        <v>143</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="O17" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P17" s="6">
-        <v>45389</v>
-      </c>
-      <c r="Q17" s="6">
-        <v>45515</v>
-      </c>
-      <c r="R17" s="7"/>
+      <c r="P17" s="5">
+        <v>45472</v>
+      </c>
+      <c r="Q17" s="5">
+        <v>45484</v>
+      </c>
+      <c r="R17" s="2"/>
       <c r="S17" s="3" t="s">
         <v>248</v>
       </c>
       <c r="T17" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="U17" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="V17" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="U17" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="V17" s="3" t="s">
+      <c r="W17" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="W17" s="3" t="s">
+      <c r="X17" s="3" t="s">
         <v>318</v>
-      </c>
-      <c r="X17" s="3" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.3">
@@ -2996,38 +3059,38 @@
         <v>15</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>125</v>
+        <v>146</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="O18" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P18" s="6">
-        <v>45372</v>
-      </c>
-      <c r="Q18" s="6">
-        <v>45383</v>
-      </c>
-      <c r="R18" s="7"/>
+      <c r="P18" s="5">
+        <v>45397</v>
+      </c>
+      <c r="Q18" s="5">
+        <v>45553</v>
+      </c>
+      <c r="R18" s="2"/>
       <c r="S18" s="3" t="s">
         <v>249</v>
       </c>
       <c r="T18" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="U18" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="V18" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="U18" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="V18" s="3" t="s">
+      <c r="W18" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="W18" s="3" t="s">
+      <c r="X18" s="3" t="s">
         <v>322</v>
-      </c>
-      <c r="X18" s="3" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.3">
@@ -3062,38 +3125,38 @@
         <v>4</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="O19" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P19" s="6">
-        <v>45310</v>
-      </c>
-      <c r="Q19" s="6">
-        <v>45351</v>
-      </c>
-      <c r="R19" s="7"/>
+      <c r="P19" s="5">
+        <v>45379</v>
+      </c>
+      <c r="Q19" s="5">
+        <v>45538</v>
+      </c>
+      <c r="R19" s="2"/>
       <c r="S19" s="3" t="s">
         <v>251</v>
       </c>
       <c r="T19" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="U19" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="V19" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="U19" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="V19" s="3" t="s">
+      <c r="W19" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="W19" s="3" t="s">
+      <c r="X19" s="3" t="s">
         <v>326</v>
-      </c>
-      <c r="X19" s="3" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.3">
@@ -3128,38 +3191,38 @@
         <v>14</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>131</v>
+        <v>149</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="O20" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P20" s="6">
-        <v>45295</v>
-      </c>
-      <c r="Q20" s="6">
-        <v>45358</v>
-      </c>
-      <c r="R20" s="7"/>
+      <c r="P20" s="5">
+        <v>45484</v>
+      </c>
+      <c r="Q20" s="5">
+        <v>45520</v>
+      </c>
+      <c r="R20" s="2"/>
       <c r="S20" s="3" t="s">
         <v>252</v>
       </c>
       <c r="T20" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="U20" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="V20" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="U20" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="V20" s="3" t="s">
+      <c r="W20" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="W20" s="3" t="s">
+      <c r="X20" s="3" t="s">
         <v>330</v>
-      </c>
-      <c r="X20" s="3" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.3">
@@ -3194,38 +3257,38 @@
         <v>4</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="N21" s="3" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="O21" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P21" s="6">
-        <v>45306</v>
-      </c>
-      <c r="Q21" s="6">
-        <v>45460</v>
-      </c>
-      <c r="R21" s="7"/>
+      <c r="P21" s="5">
+        <v>45494</v>
+      </c>
+      <c r="Q21" s="5">
+        <v>45508</v>
+      </c>
+      <c r="R21" s="2"/>
       <c r="S21" s="3" t="s">
         <v>253</v>
       </c>
       <c r="T21" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="U21" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="V21" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="U21" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="V21" s="3" t="s">
+      <c r="W21" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="W21" s="3" t="s">
+      <c r="X21" s="3" t="s">
         <v>334</v>
-      </c>
-      <c r="X21" s="3" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.3">
@@ -3260,21 +3323,21 @@
         <v>8</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>113</v>
+        <v>152</v>
       </c>
       <c r="N22" s="3" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="O22" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P22" s="6">
-        <v>45539</v>
-      </c>
-      <c r="Q22" s="6">
-        <v>45552</v>
-      </c>
-      <c r="R22" s="7"/>
+      <c r="P22" s="5">
+        <v>45472</v>
+      </c>
+      <c r="Q22" s="5">
+        <v>45520</v>
+      </c>
+      <c r="R22" s="2"/>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
@@ -3308,21 +3371,21 @@
         <v>12</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>113</v>
+        <v>155</v>
       </c>
       <c r="N23" s="3" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="O23" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P23" s="6">
-        <v>45480</v>
-      </c>
-      <c r="Q23" s="6">
-        <v>45515</v>
-      </c>
-      <c r="R23" s="7"/>
+      <c r="P23" s="5">
+        <v>45407</v>
+      </c>
+      <c r="Q23" s="5">
+        <v>45452</v>
+      </c>
+      <c r="R23" s="2"/>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
@@ -3356,21 +3419,21 @@
         <v>6</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>143</v>
+        <v>158</v>
       </c>
       <c r="N24" s="3" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="O24" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P24" s="6">
-        <v>45472</v>
-      </c>
-      <c r="Q24" s="6">
-        <v>45484</v>
-      </c>
-      <c r="R24" s="7"/>
+      <c r="P24" s="5">
+        <v>45312</v>
+      </c>
+      <c r="Q24" s="5">
+        <v>45490</v>
+      </c>
+      <c r="R24" s="2"/>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
@@ -3404,21 +3467,21 @@
         <v>11</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
       <c r="N25" s="3" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="O25" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P25" s="6">
-        <v>45397</v>
-      </c>
-      <c r="Q25" s="6">
-        <v>45553</v>
-      </c>
-      <c r="R25" s="7"/>
+      <c r="P25" s="5">
+        <v>45393</v>
+      </c>
+      <c r="Q25" s="5">
+        <v>45415</v>
+      </c>
+      <c r="R25" s="2"/>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
@@ -3452,21 +3515,21 @@
         <v>4</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>131</v>
+        <v>164</v>
       </c>
       <c r="N26" s="3" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="O26" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P26" s="6">
-        <v>45379</v>
-      </c>
-      <c r="Q26" s="6">
-        <v>45538</v>
-      </c>
-      <c r="R26" s="7"/>
+      <c r="P26" s="5">
+        <v>45430</v>
+      </c>
+      <c r="Q26" s="5">
+        <v>45476</v>
+      </c>
+      <c r="R26" s="2"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
@@ -3500,21 +3563,21 @@
         <v>14</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="N27" s="3" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="O27" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P27" s="6">
-        <v>45484</v>
-      </c>
-      <c r="Q27" s="6">
-        <v>45520</v>
-      </c>
-      <c r="R27" s="7"/>
+      <c r="P27" s="5">
+        <v>45431</v>
+      </c>
+      <c r="Q27" s="5">
+        <v>45461</v>
+      </c>
+      <c r="R27" s="2"/>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
@@ -3548,21 +3611,21 @@
         <v>3</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>146</v>
+        <v>116</v>
       </c>
       <c r="N28" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="O28" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P28" s="6">
-        <v>45494</v>
-      </c>
-      <c r="Q28" s="6">
-        <v>45508</v>
-      </c>
-      <c r="R28" s="7"/>
+      <c r="P28" s="5">
+        <v>45384</v>
+      </c>
+      <c r="Q28" s="5">
+        <v>45411</v>
+      </c>
+      <c r="R28" s="2"/>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
@@ -3596,21 +3659,21 @@
         <v>1</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>152</v>
+        <v>170</v>
       </c>
       <c r="N29" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="O29" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P29" s="6">
-        <v>45472</v>
-      </c>
-      <c r="Q29" s="6">
-        <v>45520</v>
-      </c>
-      <c r="R29" s="7"/>
+      <c r="P29" s="5">
+        <v>45314</v>
+      </c>
+      <c r="Q29" s="5">
+        <v>45390</v>
+      </c>
+      <c r="R29" s="2"/>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
@@ -3644,21 +3707,21 @@
         <v>12</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>155</v>
+        <v>173</v>
       </c>
       <c r="N30" s="3" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="O30" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P30" s="6">
-        <v>45407</v>
-      </c>
-      <c r="Q30" s="6">
-        <v>45452</v>
-      </c>
-      <c r="R30" s="7"/>
+      <c r="P30" s="5">
+        <v>45540</v>
+      </c>
+      <c r="Q30" s="5">
+        <v>45553</v>
+      </c>
+      <c r="R30" s="2"/>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
@@ -3692,21 +3755,21 @@
         <v>9</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="N31" s="3" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="O31" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P31" s="6">
-        <v>45312</v>
-      </c>
-      <c r="Q31" s="6">
-        <v>45490</v>
-      </c>
-      <c r="R31" s="7"/>
+      <c r="P31" s="5">
+        <v>45328</v>
+      </c>
+      <c r="Q31" s="5">
+        <v>45353</v>
+      </c>
+      <c r="R31" s="2"/>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
@@ -3740,21 +3803,21 @@
         <v>8</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="N32" s="3" t="s">
-        <v>235</v>
+        <v>250</v>
       </c>
       <c r="O32" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P32" s="6">
-        <v>45393</v>
-      </c>
-      <c r="Q32" s="6">
-        <v>45415</v>
-      </c>
-      <c r="R32" s="7"/>
+      <c r="P32" s="5">
+        <v>45538</v>
+      </c>
+      <c r="Q32" s="5">
+        <v>45557</v>
+      </c>
+      <c r="R32" s="2"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
@@ -3788,21 +3851,21 @@
         <v>8</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>164</v>
+        <v>122</v>
       </c>
       <c r="N33" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="O33" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P33" s="6">
-        <v>45430</v>
-      </c>
-      <c r="Q33" s="6">
-        <v>45476</v>
-      </c>
-      <c r="R33" s="7"/>
+      <c r="P33" s="5">
+        <v>45555</v>
+      </c>
+      <c r="Q33" s="5">
+        <v>45557</v>
+      </c>
+      <c r="R33" s="2"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
@@ -3836,21 +3899,21 @@
         <v>9</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>167</v>
+        <v>110</v>
       </c>
       <c r="N34" s="3" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="O34" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P34" s="6">
-        <v>45431</v>
-      </c>
-      <c r="Q34" s="6">
-        <v>45461</v>
-      </c>
-      <c r="R34" s="7"/>
+      <c r="P34" s="5">
+        <v>45339</v>
+      </c>
+      <c r="Q34" s="5">
+        <v>45418</v>
+      </c>
+      <c r="R34" s="2"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
@@ -3884,21 +3947,21 @@
         <v>5</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>116</v>
+        <v>182</v>
       </c>
       <c r="N35" s="3" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
       <c r="O35" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P35" s="6">
-        <v>45384</v>
-      </c>
-      <c r="Q35" s="6">
-        <v>45411</v>
-      </c>
-      <c r="R35" s="7"/>
+      <c r="P35" s="5">
+        <v>45409</v>
+      </c>
+      <c r="Q35" s="5">
+        <v>45511</v>
+      </c>
+      <c r="R35" s="2"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
@@ -3932,21 +3995,21 @@
         <v>7</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="N36" s="3" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="O36" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P36" s="6">
-        <v>45314</v>
-      </c>
-      <c r="Q36" s="6">
-        <v>45390</v>
-      </c>
-      <c r="R36" s="7"/>
+      <c r="P36" s="5">
+        <v>45493</v>
+      </c>
+      <c r="Q36" s="5">
+        <v>45513</v>
+      </c>
+      <c r="R36" s="2"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
@@ -3980,21 +4043,21 @@
         <v>6</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>173</v>
+        <v>188</v>
       </c>
       <c r="N37" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="O37" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P37" s="6">
-        <v>45540</v>
-      </c>
-      <c r="Q37" s="6">
-        <v>45553</v>
-      </c>
-      <c r="R37" s="7"/>
+      <c r="P37" s="5">
+        <v>45300</v>
+      </c>
+      <c r="Q37" s="5">
+        <v>45492</v>
+      </c>
+      <c r="R37" s="2"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
@@ -4028,21 +4091,21 @@
         <v>5</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>179</v>
+        <v>131</v>
       </c>
       <c r="N38" s="3" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="O38" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P38" s="6">
-        <v>45328</v>
-      </c>
-      <c r="Q38" s="6">
-        <v>45353</v>
-      </c>
-      <c r="R38" s="7"/>
+      <c r="P38" s="5">
+        <v>45522</v>
+      </c>
+      <c r="Q38" s="5">
+        <v>45522</v>
+      </c>
+      <c r="R38" s="2"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
@@ -4076,21 +4139,21 @@
         <v>8</v>
       </c>
       <c r="M39" s="3" t="s">
-        <v>146</v>
+        <v>113</v>
       </c>
       <c r="N39" s="3" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="O39" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P39" s="6">
-        <v>45538</v>
-      </c>
-      <c r="Q39" s="6">
-        <v>45557</v>
-      </c>
-      <c r="R39" s="7"/>
+      <c r="P39" s="5">
+        <v>45309</v>
+      </c>
+      <c r="Q39" s="5">
+        <v>45536</v>
+      </c>
+      <c r="R39" s="2"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
@@ -4124,21 +4187,21 @@
         <v>11</v>
       </c>
       <c r="M40" s="3" t="s">
-        <v>122</v>
+        <v>179</v>
       </c>
       <c r="N40" s="3" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="O40" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P40" s="6">
-        <v>45555</v>
-      </c>
-      <c r="Q40" s="6">
-        <v>45557</v>
-      </c>
-      <c r="R40" s="7"/>
+      <c r="P40" s="5">
+        <v>45397</v>
+      </c>
+      <c r="Q40" s="5">
+        <v>45535</v>
+      </c>
+      <c r="R40" s="2"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
@@ -4172,21 +4235,21 @@
         <v>12</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>110</v>
+        <v>191</v>
       </c>
       <c r="N41" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="O41" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P41" s="6">
-        <v>45339</v>
-      </c>
-      <c r="Q41" s="6">
-        <v>45418</v>
-      </c>
-      <c r="R41" s="7"/>
+      <c r="P41" s="5">
+        <v>45395</v>
+      </c>
+      <c r="Q41" s="5">
+        <v>45551</v>
+      </c>
+      <c r="R41" s="2"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
@@ -4220,21 +4283,21 @@
         <v>2</v>
       </c>
       <c r="M42" s="3" t="s">
-        <v>182</v>
+        <v>119</v>
       </c>
       <c r="N42" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="O42" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P42" s="6">
-        <v>45409</v>
-      </c>
-      <c r="Q42" s="6">
-        <v>45511</v>
-      </c>
-      <c r="R42" s="7"/>
+      <c r="P42" s="5">
+        <v>45448</v>
+      </c>
+      <c r="Q42" s="5">
+        <v>45527</v>
+      </c>
+      <c r="R42" s="2"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
@@ -4268,21 +4331,21 @@
         <v>12</v>
       </c>
       <c r="M43" s="3" t="s">
-        <v>152</v>
+        <v>97</v>
       </c>
       <c r="N43" s="3" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="O43" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P43" s="6">
-        <v>45493</v>
-      </c>
-      <c r="Q43" s="6">
-        <v>45513</v>
-      </c>
-      <c r="R43" s="7"/>
+      <c r="P43" s="5">
+        <v>45422</v>
+      </c>
+      <c r="Q43" s="5">
+        <v>45498</v>
+      </c>
+      <c r="R43" s="2"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
@@ -4316,21 +4379,21 @@
         <v>4</v>
       </c>
       <c r="M44" s="3" t="s">
-        <v>188</v>
+        <v>143</v>
       </c>
       <c r="N44" s="3" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="O44" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P44" s="6">
-        <v>45300</v>
-      </c>
-      <c r="Q44" s="6">
-        <v>45492</v>
-      </c>
-      <c r="R44" s="7"/>
+      <c r="P44" s="5">
+        <v>45325</v>
+      </c>
+      <c r="Q44" s="5">
+        <v>45382</v>
+      </c>
+      <c r="R44" s="2"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
@@ -4364,21 +4427,21 @@
         <v>12</v>
       </c>
       <c r="M45" s="3" t="s">
-        <v>131</v>
+        <v>155</v>
       </c>
       <c r="N45" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="O45" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P45" s="6">
-        <v>45522</v>
-      </c>
-      <c r="Q45" s="6">
-        <v>45522</v>
-      </c>
-      <c r="R45" s="7"/>
+      <c r="P45" s="5">
+        <v>45317</v>
+      </c>
+      <c r="Q45" s="5">
+        <v>45355</v>
+      </c>
+      <c r="R45" s="2"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
@@ -4412,562 +4475,562 @@
         <v>11</v>
       </c>
       <c r="M46" s="3" t="s">
-        <v>113</v>
+        <v>164</v>
       </c>
       <c r="N46" s="3" t="s">
-        <v>236</v>
+        <v>252</v>
       </c>
       <c r="O46" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P46" s="6">
-        <v>45309</v>
-      </c>
-      <c r="Q46" s="6">
-        <v>45536</v>
-      </c>
-      <c r="R46" s="7"/>
+      <c r="P46" s="5">
+        <v>45360</v>
+      </c>
+      <c r="Q46" s="5">
+        <v>45443</v>
+      </c>
+      <c r="R46" s="2"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C47" s="1"/>
       <c r="M47" s="3" t="s">
-        <v>179</v>
+        <v>197</v>
       </c>
       <c r="N47" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O47" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P47" s="6">
-        <v>45397</v>
-      </c>
-      <c r="Q47" s="6">
-        <v>45535</v>
-      </c>
-      <c r="R47" s="7"/>
+      <c r="P47" s="5">
+        <v>45399</v>
+      </c>
+      <c r="Q47" s="5">
+        <v>45523</v>
+      </c>
+      <c r="R47" s="2"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="M48" s="3" t="s">
-        <v>191</v>
+        <v>119</v>
       </c>
       <c r="N48" s="3" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="O48" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P48" s="6">
-        <v>45395</v>
-      </c>
-      <c r="Q48" s="6">
-        <v>45551</v>
-      </c>
-      <c r="R48" s="7"/>
+      <c r="P48" s="5">
+        <v>45295</v>
+      </c>
+      <c r="Q48" s="5">
+        <v>45434</v>
+      </c>
+      <c r="R48" s="2"/>
     </row>
     <row r="49" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M49" s="3" t="s">
-        <v>119</v>
+        <v>152</v>
       </c>
       <c r="N49" s="3" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="O49" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P49" s="6">
-        <v>45448</v>
-      </c>
-      <c r="Q49" s="6">
-        <v>45527</v>
-      </c>
-      <c r="R49" s="7"/>
+      <c r="P49" s="5">
+        <v>45538</v>
+      </c>
+      <c r="Q49" s="5">
+        <v>45549</v>
+      </c>
+      <c r="R49" s="2"/>
     </row>
     <row r="50" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M50" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="N50" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="O50" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P50" s="6">
-        <v>45422</v>
-      </c>
-      <c r="Q50" s="6">
-        <v>45498</v>
-      </c>
-      <c r="R50" s="7"/>
+      <c r="P50" s="5">
+        <v>45310</v>
+      </c>
+      <c r="Q50" s="5">
+        <v>45456</v>
+      </c>
+      <c r="R50" s="2"/>
     </row>
     <row r="51" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M51" s="3" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="N51" s="3" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="O51" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P51" s="6">
-        <v>45325</v>
-      </c>
-      <c r="Q51" s="6">
-        <v>45382</v>
-      </c>
-      <c r="R51" s="7"/>
+      <c r="P51" s="5">
+        <v>45376</v>
+      </c>
+      <c r="Q51" s="5">
+        <v>45551</v>
+      </c>
+      <c r="R51" s="2"/>
     </row>
     <row r="52" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M52" s="3" t="s">
-        <v>155</v>
+        <v>200</v>
       </c>
       <c r="N52" s="3" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="O52" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P52" s="6">
-        <v>45317</v>
-      </c>
-      <c r="Q52" s="6">
-        <v>45355</v>
-      </c>
-      <c r="R52" s="7"/>
+      <c r="P52" s="5">
+        <v>45426</v>
+      </c>
+      <c r="Q52" s="5">
+        <v>45548</v>
+      </c>
+      <c r="R52" s="2"/>
     </row>
     <row r="53" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M53" s="3" t="s">
-        <v>164</v>
+        <v>188</v>
       </c>
       <c r="N53" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="O53" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P53" s="6">
-        <v>45360</v>
-      </c>
-      <c r="Q53" s="6">
-        <v>45443</v>
-      </c>
-      <c r="R53" s="7"/>
+      <c r="P53" s="5">
+        <v>45369</v>
+      </c>
+      <c r="Q53" s="5">
+        <v>45405</v>
+      </c>
+      <c r="R53" s="2"/>
     </row>
     <row r="54" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M54" s="3" t="s">
-        <v>197</v>
+        <v>128</v>
       </c>
       <c r="N54" s="3" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="O54" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P54" s="6">
-        <v>45399</v>
-      </c>
-      <c r="Q54" s="6">
-        <v>45523</v>
-      </c>
-      <c r="R54" s="7"/>
+      <c r="P54" s="5">
+        <v>45400</v>
+      </c>
+      <c r="Q54" s="5">
+        <v>45404</v>
+      </c>
+      <c r="R54" s="2"/>
     </row>
     <row r="55" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M55" s="3" t="s">
-        <v>119</v>
+        <v>149</v>
       </c>
       <c r="N55" s="3" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="O55" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P55" s="6">
-        <v>45295</v>
-      </c>
-      <c r="Q55" s="6">
-        <v>45434</v>
-      </c>
-      <c r="R55" s="7"/>
+      <c r="P55" s="5">
+        <v>45330</v>
+      </c>
+      <c r="Q55" s="5">
+        <v>45397</v>
+      </c>
+      <c r="R55" s="2"/>
     </row>
     <row r="56" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M56" s="3" t="s">
-        <v>152</v>
+        <v>110</v>
       </c>
       <c r="N56" s="3" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="O56" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P56" s="6">
-        <v>45538</v>
-      </c>
-      <c r="Q56" s="6">
-        <v>45549</v>
-      </c>
-      <c r="R56" s="7"/>
+      <c r="P56" s="5">
+        <v>45362</v>
+      </c>
+      <c r="Q56" s="5">
+        <v>45491</v>
+      </c>
+      <c r="R56" s="2"/>
     </row>
     <row r="57" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M57" s="3" t="s">
-        <v>104</v>
+        <v>209</v>
       </c>
       <c r="N57" s="3" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="O57" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P57" s="6">
-        <v>45310</v>
-      </c>
-      <c r="Q57" s="6">
-        <v>45456</v>
-      </c>
-      <c r="R57" s="7"/>
+      <c r="P57" s="5">
+        <v>45480</v>
+      </c>
+      <c r="Q57" s="5">
+        <v>45530</v>
+      </c>
+      <c r="R57" s="2"/>
     </row>
     <row r="58" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M58" s="3" t="s">
-        <v>116</v>
+        <v>143</v>
       </c>
       <c r="N58" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O58" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P58" s="6">
-        <v>45376</v>
-      </c>
-      <c r="Q58" s="6">
-        <v>45551</v>
-      </c>
-      <c r="R58" s="7"/>
+      <c r="P58" s="5">
+        <v>45461</v>
+      </c>
+      <c r="Q58" s="5">
+        <v>45504</v>
+      </c>
+      <c r="R58" s="2"/>
     </row>
     <row r="59" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M59" s="3" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="N59" s="3" t="s">
-        <v>235</v>
+        <v>248</v>
       </c>
       <c r="O59" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P59" s="6">
-        <v>45426</v>
-      </c>
-      <c r="Q59" s="6">
-        <v>45548</v>
-      </c>
-      <c r="R59" s="7"/>
+      <c r="P59" s="5">
+        <v>45410</v>
+      </c>
+      <c r="Q59" s="5">
+        <v>45485</v>
+      </c>
+      <c r="R59" s="2"/>
     </row>
     <row r="60" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M60" s="3" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="N60" s="3" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="O60" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P60" s="6">
-        <v>45369</v>
-      </c>
-      <c r="Q60" s="6">
-        <v>45405</v>
-      </c>
-      <c r="R60" s="7"/>
+      <c r="P60" s="5">
+        <v>45335</v>
+      </c>
+      <c r="Q60" s="5">
+        <v>45340</v>
+      </c>
+      <c r="R60" s="2"/>
     </row>
     <row r="61" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M61" s="3" t="s">
-        <v>128</v>
+        <v>101</v>
       </c>
       <c r="N61" s="3" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="O61" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P61" s="6">
-        <v>45400</v>
-      </c>
-      <c r="Q61" s="6">
-        <v>45404</v>
-      </c>
-      <c r="R61" s="7"/>
+      <c r="P61" s="5">
+        <v>45514</v>
+      </c>
+      <c r="Q61" s="5">
+        <v>45543</v>
+      </c>
+      <c r="R61" s="2"/>
     </row>
     <row r="62" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M62" s="3" t="s">
-        <v>149</v>
+        <v>218</v>
       </c>
       <c r="N62" s="3" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="O62" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P62" s="6">
-        <v>45330</v>
-      </c>
-      <c r="Q62" s="6">
-        <v>45397</v>
-      </c>
-      <c r="R62" s="7"/>
+      <c r="P62" s="5">
+        <v>45531</v>
+      </c>
+      <c r="Q62" s="5">
+        <v>45532</v>
+      </c>
+      <c r="R62" s="2"/>
     </row>
     <row r="63" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M63" s="3" t="s">
-        <v>110</v>
+        <v>221</v>
       </c>
       <c r="N63" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="O63" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P63" s="6">
-        <v>45362</v>
-      </c>
-      <c r="Q63" s="6">
-        <v>45491</v>
-      </c>
-      <c r="R63" s="7"/>
+      <c r="P63" s="5">
+        <v>45368</v>
+      </c>
+      <c r="Q63" s="5">
+        <v>45398</v>
+      </c>
+      <c r="R63" s="2"/>
     </row>
     <row r="64" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M64" s="3" t="s">
-        <v>209</v>
+        <v>143</v>
       </c>
       <c r="N64" s="3" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="O64" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P64" s="6">
-        <v>45480</v>
-      </c>
-      <c r="Q64" s="6">
-        <v>45530</v>
-      </c>
-      <c r="R64" s="7"/>
+      <c r="P64" s="5">
+        <v>45365</v>
+      </c>
+      <c r="Q64" s="5">
+        <v>45395</v>
+      </c>
+      <c r="R64" s="2"/>
     </row>
     <row r="65" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M65" s="3" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="N65" s="3" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="O65" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P65" s="6">
-        <v>45461</v>
-      </c>
-      <c r="Q65" s="6">
-        <v>45504</v>
-      </c>
-      <c r="R65" s="7"/>
+      <c r="P65" s="5">
+        <v>45409</v>
+      </c>
+      <c r="Q65" s="5">
+        <v>45541</v>
+      </c>
+      <c r="R65" s="2"/>
     </row>
     <row r="66" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M66" s="3" t="s">
-        <v>212</v>
+        <v>170</v>
       </c>
       <c r="N66" s="3" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="O66" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P66" s="6">
-        <v>45410</v>
-      </c>
-      <c r="Q66" s="6">
-        <v>45485</v>
-      </c>
-      <c r="R66" s="7"/>
+      <c r="P66" s="5">
+        <v>45462</v>
+      </c>
+      <c r="Q66" s="5">
+        <v>45506</v>
+      </c>
+      <c r="R66" s="2"/>
     </row>
     <row r="67" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M67" s="3" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="N67" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="O67" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P67" s="6">
-        <v>45335</v>
-      </c>
-      <c r="Q67" s="6">
-        <v>45340</v>
-      </c>
-      <c r="R67" s="7"/>
+      <c r="P67" s="5">
+        <v>45521</v>
+      </c>
+      <c r="Q67" s="5">
+        <v>45554</v>
+      </c>
+      <c r="R67" s="2"/>
     </row>
     <row r="68" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M68" s="3" t="s">
         <v>101</v>
       </c>
       <c r="N68" s="3" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="O68" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P68" s="6">
-        <v>45514</v>
-      </c>
-      <c r="Q68" s="6">
-        <v>45543</v>
-      </c>
-      <c r="R68" s="7"/>
+      <c r="P68" s="5">
+        <v>45369</v>
+      </c>
+      <c r="Q68" s="5">
+        <v>45437</v>
+      </c>
+      <c r="R68" s="2"/>
     </row>
     <row r="69" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M69" s="3" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="N69" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="O69" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P69" s="6">
-        <v>45531</v>
-      </c>
-      <c r="Q69" s="6">
-        <v>45532</v>
-      </c>
-      <c r="R69" s="7"/>
+      <c r="P69" s="5">
+        <v>45513</v>
+      </c>
+      <c r="Q69" s="5">
+        <v>45521</v>
+      </c>
+      <c r="R69" s="2"/>
     </row>
     <row r="70" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M70" s="3" t="s">
         <v>221</v>
       </c>
       <c r="N70" s="3" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="O70" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P70" s="6">
-        <v>45368</v>
-      </c>
-      <c r="Q70" s="6">
-        <v>45398</v>
-      </c>
-      <c r="R70" s="7"/>
+      <c r="P70" s="5">
+        <v>45330</v>
+      </c>
+      <c r="Q70" s="5">
+        <v>45383</v>
+      </c>
+      <c r="R70" s="2"/>
     </row>
     <row r="71" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M71" s="3" t="s">
-        <v>143</v>
+        <v>182</v>
       </c>
       <c r="N71" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="O71" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P71" s="6">
-        <v>45365</v>
-      </c>
-      <c r="Q71" s="6">
-        <v>45395</v>
-      </c>
-      <c r="R71" s="7"/>
+      <c r="P71" s="5">
+        <v>45350</v>
+      </c>
+      <c r="Q71" s="5">
+        <v>45517</v>
+      </c>
+      <c r="R71" s="2"/>
     </row>
     <row r="72" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M72" s="3" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="N72" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="O72" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P72" s="6">
-        <v>45409</v>
-      </c>
-      <c r="Q72" s="6">
-        <v>45541</v>
-      </c>
-      <c r="R72" s="7"/>
+      <c r="P72" s="5">
+        <v>45410</v>
+      </c>
+      <c r="Q72" s="5">
+        <v>45433</v>
+      </c>
+      <c r="R72" s="2"/>
     </row>
     <row r="73" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M73" s="3" t="s">
-        <v>170</v>
+        <v>227</v>
       </c>
       <c r="N73" s="3" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="O73" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P73" s="6">
-        <v>45462</v>
-      </c>
-      <c r="Q73" s="6">
-        <v>45506</v>
-      </c>
-      <c r="R73" s="7"/>
+      <c r="P73" s="5">
+        <v>45318</v>
+      </c>
+      <c r="Q73" s="5">
+        <v>45322</v>
+      </c>
+      <c r="R73" s="2"/>
     </row>
     <row r="74" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M74" s="3" t="s">
-        <v>227</v>
+        <v>97</v>
       </c>
       <c r="N74" s="3" t="s">
-        <v>241</v>
+        <v>252</v>
       </c>
       <c r="O74" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P74" s="6">
-        <v>45521</v>
-      </c>
-      <c r="Q74" s="6">
-        <v>45554</v>
-      </c>
-      <c r="R74" s="7"/>
+      <c r="P74" s="5">
+        <v>45520</v>
+      </c>
+      <c r="Q74" s="5">
+        <v>45523</v>
+      </c>
+      <c r="R74" s="2"/>
     </row>
     <row r="75" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M75" s="3" t="s">
-        <v>101</v>
+        <v>212</v>
       </c>
       <c r="N75" s="3" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="O75" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P75" s="6">
-        <v>45369</v>
-      </c>
-      <c r="Q75" s="6">
-        <v>45437</v>
-      </c>
-      <c r="R75" s="7"/>
+      <c r="P75" s="5">
+        <v>45486</v>
+      </c>
+      <c r="Q75" s="5">
+        <v>45532</v>
+      </c>
+      <c r="R75" s="2"/>
     </row>
     <row r="76" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M76" s="3" t="s">
         <v>221</v>
       </c>
       <c r="N76" s="3" t="s">
-        <v>238</v>
+        <v>248</v>
       </c>
       <c r="O76" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P76" s="6">
-        <v>45513</v>
-      </c>
-      <c r="Q76" s="6">
-        <v>45521</v>
-      </c>
-      <c r="R76" s="7"/>
+      <c r="P76" s="5">
+        <v>45510</v>
+      </c>
+      <c r="Q76" s="5">
+        <v>45532</v>
+      </c>
+      <c r="R76" s="2"/>
     </row>
     <row r="77" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M77" s="3" t="s">
@@ -4979,35 +5042,35 @@
       <c r="O77" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P77" s="6">
-        <v>45330</v>
-      </c>
-      <c r="Q77" s="6">
-        <v>45383</v>
-      </c>
-      <c r="R77" s="7"/>
+      <c r="P77" s="5">
+        <v>45546</v>
+      </c>
+      <c r="Q77" s="5">
+        <v>45553</v>
+      </c>
+      <c r="R77" s="2"/>
     </row>
     <row r="78" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M78" s="3" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="N78" s="3" t="s">
-        <v>240</v>
+        <v>253</v>
       </c>
       <c r="O78" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P78" s="6">
-        <v>45350</v>
-      </c>
-      <c r="Q78" s="6">
-        <v>45517</v>
-      </c>
-      <c r="R78" s="7"/>
+      <c r="P78" s="5">
+        <v>45355</v>
+      </c>
+      <c r="Q78" s="5">
+        <v>45512</v>
+      </c>
+      <c r="R78" s="2"/>
     </row>
     <row r="79" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M79" s="3" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="N79" s="3" t="s">
         <v>242</v>
@@ -5015,546 +5078,427 @@
       <c r="O79" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P79" s="6">
-        <v>45410</v>
-      </c>
-      <c r="Q79" s="6">
-        <v>45433</v>
-      </c>
-      <c r="R79" s="7"/>
+      <c r="P79" s="5">
+        <v>45401</v>
+      </c>
+      <c r="Q79" s="5">
+        <v>45469</v>
+      </c>
+      <c r="R79" s="2"/>
     </row>
     <row r="80" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M80" s="3" t="s">
-        <v>227</v>
+        <v>107</v>
       </c>
       <c r="N80" s="3" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
       <c r="O80" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P80" s="6">
-        <v>45318</v>
-      </c>
-      <c r="Q80" s="6">
-        <v>45322</v>
-      </c>
-      <c r="R80" s="7"/>
+      <c r="P80" s="5">
+        <v>45325</v>
+      </c>
+      <c r="Q80" s="5">
+        <v>45490</v>
+      </c>
+      <c r="R80" s="2"/>
     </row>
     <row r="81" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M81" s="3" t="s">
-        <v>97</v>
+        <v>137</v>
       </c>
       <c r="N81" s="3" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
       <c r="O81" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P81" s="6">
-        <v>45520</v>
-      </c>
-      <c r="Q81" s="6">
-        <v>45523</v>
-      </c>
-      <c r="R81" s="7"/>
+      <c r="P81" s="5">
+        <v>45463</v>
+      </c>
+      <c r="Q81" s="5">
+        <v>45504</v>
+      </c>
+      <c r="R81" s="2"/>
     </row>
     <row r="82" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M82" s="3" t="s">
-        <v>212</v>
+        <v>140</v>
       </c>
       <c r="N82" s="3" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="O82" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P82" s="6">
-        <v>45486</v>
-      </c>
-      <c r="Q82" s="6">
-        <v>45532</v>
-      </c>
-      <c r="R82" s="7"/>
+      <c r="P82" s="5">
+        <v>45551</v>
+      </c>
+      <c r="Q82" s="5">
+        <v>45551</v>
+      </c>
+      <c r="R82" s="2"/>
     </row>
     <row r="83" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M83" s="3" t="s">
-        <v>221</v>
+        <v>176</v>
       </c>
       <c r="N83" s="3" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="O83" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P83" s="6">
-        <v>45510</v>
-      </c>
-      <c r="Q83" s="6">
-        <v>45532</v>
-      </c>
-      <c r="R83" s="7"/>
+      <c r="P83" s="5">
+        <v>45416</v>
+      </c>
+      <c r="Q83" s="5">
+        <v>45416</v>
+      </c>
+      <c r="R83" s="2"/>
     </row>
     <row r="84" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M84" s="3" t="s">
-        <v>221</v>
+        <v>107</v>
       </c>
       <c r="N84" s="3" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="O84" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P84" s="6">
-        <v>45546</v>
-      </c>
-      <c r="Q84" s="6">
-        <v>45553</v>
-      </c>
-      <c r="R84" s="7"/>
+      <c r="P84" s="5">
+        <v>45360</v>
+      </c>
+      <c r="Q84" s="5">
+        <v>45468</v>
+      </c>
+      <c r="R84" s="2"/>
     </row>
     <row r="85" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M85" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="N85" s="3" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="O85" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P85" s="6">
-        <v>45355</v>
-      </c>
-      <c r="Q85" s="6">
-        <v>45512</v>
-      </c>
-      <c r="R85" s="7"/>
+      <c r="P85" s="5">
+        <v>45440</v>
+      </c>
+      <c r="Q85" s="5">
+        <v>45482</v>
+      </c>
+      <c r="R85" s="2"/>
     </row>
     <row r="86" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M86" s="3" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
       <c r="N86" s="3" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="O86" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P86" s="6">
-        <v>45401</v>
-      </c>
-      <c r="Q86" s="6">
-        <v>45469</v>
-      </c>
-      <c r="R86" s="7"/>
+      <c r="P86" s="5">
+        <v>45409</v>
+      </c>
+      <c r="Q86" s="5">
+        <v>45496</v>
+      </c>
+      <c r="R86" s="2"/>
     </row>
     <row r="87" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M87" s="3" t="s">
-        <v>107</v>
+        <v>194</v>
       </c>
       <c r="N87" s="3" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
       <c r="O87" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P87" s="6">
-        <v>45325</v>
-      </c>
-      <c r="Q87" s="6">
-        <v>45490</v>
-      </c>
-      <c r="R87" s="7"/>
+      <c r="P87" s="5">
+        <v>45476</v>
+      </c>
+      <c r="Q87" s="5">
+        <v>45557</v>
+      </c>
+      <c r="R87" s="2"/>
     </row>
     <row r="88" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M88" s="3" t="s">
-        <v>137</v>
+        <v>107</v>
       </c>
       <c r="N88" s="3" t="s">
-        <v>235</v>
+        <v>253</v>
       </c>
       <c r="O88" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P88" s="6">
-        <v>45463</v>
-      </c>
-      <c r="Q88" s="6">
-        <v>45504</v>
-      </c>
-      <c r="R88" s="7"/>
+      <c r="P88" s="5">
+        <v>45486</v>
+      </c>
+      <c r="Q88" s="5">
+        <v>45512</v>
+      </c>
+      <c r="R88" s="2"/>
     </row>
     <row r="89" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M89" s="3" t="s">
-        <v>140</v>
+        <v>203</v>
       </c>
       <c r="N89" s="3" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="O89" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P89" s="6">
-        <v>45551</v>
-      </c>
-      <c r="Q89" s="6">
-        <v>45551</v>
-      </c>
-      <c r="R89" s="7"/>
+      <c r="P89" s="5">
+        <v>45333</v>
+      </c>
+      <c r="Q89" s="5">
+        <v>45333</v>
+      </c>
+      <c r="R89" s="2"/>
     </row>
     <row r="90" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M90" s="3" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="N90" s="3" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="O90" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P90" s="6">
-        <v>45416</v>
-      </c>
-      <c r="Q90" s="6">
-        <v>45416</v>
-      </c>
-      <c r="R90" s="7"/>
+      <c r="P90" s="5">
+        <v>45470</v>
+      </c>
+      <c r="Q90" s="5">
+        <v>45550</v>
+      </c>
+      <c r="R90" s="2"/>
     </row>
     <row r="91" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M91" s="3" t="s">
-        <v>107</v>
+        <v>140</v>
       </c>
       <c r="N91" s="3" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="O91" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P91" s="6">
-        <v>45360</v>
-      </c>
-      <c r="Q91" s="6">
-        <v>45468</v>
-      </c>
-      <c r="R91" s="7"/>
+      <c r="P91" s="5">
+        <v>45476</v>
+      </c>
+      <c r="Q91" s="5">
+        <v>45546</v>
+      </c>
+      <c r="R91" s="2"/>
     </row>
     <row r="92" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M92" s="3" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="N92" s="3" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="O92" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P92" s="6">
-        <v>45440</v>
-      </c>
-      <c r="Q92" s="6">
-        <v>45482</v>
-      </c>
-      <c r="R92" s="7"/>
+      <c r="P92" s="5">
+        <v>45413</v>
+      </c>
+      <c r="Q92" s="5">
+        <v>45495</v>
+      </c>
+      <c r="R92" s="2"/>
     </row>
     <row r="93" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M93" s="3" t="s">
-        <v>137</v>
+        <v>206</v>
       </c>
       <c r="N93" s="3" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="O93" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P93" s="6">
-        <v>45409</v>
-      </c>
-      <c r="Q93" s="6">
-        <v>45496</v>
-      </c>
-      <c r="R93" s="7"/>
+      <c r="P93" s="5">
+        <v>45485</v>
+      </c>
+      <c r="Q93" s="5">
+        <v>45535</v>
+      </c>
+      <c r="R93" s="2"/>
     </row>
     <row r="94" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M94" s="3" t="s">
-        <v>194</v>
+        <v>107</v>
       </c>
       <c r="N94" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="O94" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P94" s="6">
-        <v>45476</v>
-      </c>
-      <c r="Q94" s="6">
-        <v>45557</v>
-      </c>
-      <c r="R94" s="7"/>
+      <c r="P94" s="5">
+        <v>45447</v>
+      </c>
+      <c r="Q94" s="5">
+        <v>45451</v>
+      </c>
+      <c r="R94" s="2"/>
     </row>
     <row r="95" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M95" s="3" t="s">
-        <v>107</v>
+        <v>224</v>
       </c>
       <c r="N95" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O95" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P95" s="6">
-        <v>45486</v>
-      </c>
-      <c r="Q95" s="6">
-        <v>45512</v>
-      </c>
-      <c r="R95" s="7"/>
+      <c r="P95" s="5">
+        <v>45518</v>
+      </c>
+      <c r="Q95" s="5">
+        <v>45527</v>
+      </c>
+      <c r="R95" s="2"/>
     </row>
     <row r="96" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M96" s="3" t="s">
-        <v>203</v>
+        <v>137</v>
       </c>
       <c r="N96" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="O96" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P96" s="6">
-        <v>45333</v>
-      </c>
-      <c r="Q96" s="6">
-        <v>45333</v>
-      </c>
-      <c r="R96" s="7"/>
+      <c r="P96" s="5">
+        <v>45442</v>
+      </c>
+      <c r="Q96" s="5">
+        <v>45528</v>
+      </c>
+      <c r="R96" s="2"/>
     </row>
     <row r="97" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M97" s="3" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="N97" s="3" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="O97" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P97" s="6">
-        <v>45470</v>
-      </c>
-      <c r="Q97" s="6">
-        <v>45550</v>
-      </c>
-      <c r="R97" s="7"/>
+      <c r="P97" s="5">
+        <v>45435</v>
+      </c>
+      <c r="Q97" s="5">
+        <v>45538</v>
+      </c>
+      <c r="R97" s="2"/>
     </row>
     <row r="98" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M98" s="3" t="s">
-        <v>140</v>
+        <v>194</v>
       </c>
       <c r="N98" s="3" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="O98" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P98" s="6">
-        <v>45476</v>
-      </c>
-      <c r="Q98" s="6">
-        <v>45546</v>
-      </c>
-      <c r="R98" s="7"/>
+      <c r="P98" s="5">
+        <v>45367</v>
+      </c>
+      <c r="Q98" s="5">
+        <v>45447</v>
+      </c>
+      <c r="R98" s="2"/>
     </row>
     <row r="99" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M99" s="3" t="s">
-        <v>203</v>
+        <v>185</v>
       </c>
       <c r="N99" s="3" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
       <c r="O99" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P99" s="6">
-        <v>45413</v>
-      </c>
-      <c r="Q99" s="6">
-        <v>45495</v>
-      </c>
-      <c r="R99" s="7"/>
+      <c r="P99" s="5">
+        <v>45409</v>
+      </c>
+      <c r="Q99" s="5">
+        <v>45472</v>
+      </c>
+      <c r="R99" s="2"/>
     </row>
     <row r="100" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M100" s="3" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="N100" s="3" t="s">
-        <v>236</v>
+        <v>253</v>
       </c>
       <c r="O100" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P100" s="6">
-        <v>45485</v>
-      </c>
-      <c r="Q100" s="6">
-        <v>45535</v>
-      </c>
-      <c r="R100" s="7"/>
+      <c r="P100" s="5">
+        <v>45331</v>
+      </c>
+      <c r="Q100" s="5">
+        <v>45372</v>
+      </c>
+      <c r="R100" s="2"/>
     </row>
     <row r="101" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M101" s="3" t="s">
-        <v>107</v>
+        <v>140</v>
       </c>
       <c r="N101" s="3" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="O101" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P101" s="6">
-        <v>45447</v>
-      </c>
-      <c r="Q101" s="6">
-        <v>45451</v>
-      </c>
-      <c r="R101" s="7"/>
+      <c r="P101" s="5">
+        <v>45538</v>
+      </c>
+      <c r="Q101" s="5">
+        <v>45539</v>
+      </c>
+      <c r="R101" s="2"/>
     </row>
     <row r="102" spans="13:18" x14ac:dyDescent="0.3">
       <c r="M102" s="3" t="s">
-        <v>224</v>
+        <v>176</v>
       </c>
       <c r="N102" s="3" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="O102" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P102" s="6">
-        <v>45518</v>
-      </c>
-      <c r="Q102" s="6">
-        <v>45527</v>
-      </c>
-      <c r="R102" s="7"/>
-    </row>
-    <row r="103" spans="13:18" x14ac:dyDescent="0.3">
-      <c r="M103" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="N103" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="O103" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="P103" s="6">
-        <v>45442</v>
-      </c>
-      <c r="Q103" s="6">
-        <v>45528</v>
-      </c>
-    </row>
-    <row r="104" spans="13:18" x14ac:dyDescent="0.3">
-      <c r="M104" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="N104" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="O104" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="P104" s="6">
-        <v>45435</v>
-      </c>
-      <c r="Q104" s="6">
-        <v>45538</v>
-      </c>
-    </row>
-    <row r="105" spans="13:18" x14ac:dyDescent="0.3">
-      <c r="M105" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="N105" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="O105" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="P105" s="6">
-        <v>45367</v>
-      </c>
-      <c r="Q105" s="6">
-        <v>45447</v>
-      </c>
-    </row>
-    <row r="106" spans="13:18" x14ac:dyDescent="0.3">
-      <c r="M106" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="N106" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="O106" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="P106" s="6">
-        <v>45409</v>
-      </c>
-      <c r="Q106" s="6">
-        <v>45472</v>
-      </c>
-    </row>
-    <row r="107" spans="13:18" x14ac:dyDescent="0.3">
-      <c r="M107" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="N107" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="O107" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="P107" s="6">
-        <v>45331</v>
-      </c>
-      <c r="Q107" s="6">
-        <v>45372</v>
-      </c>
-    </row>
-    <row r="108" spans="13:18" x14ac:dyDescent="0.3">
-      <c r="M108" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="N108" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="O108" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="P108" s="6">
-        <v>45538</v>
-      </c>
-      <c r="Q108" s="6">
-        <v>45539</v>
-      </c>
-    </row>
-    <row r="109" spans="13:18" x14ac:dyDescent="0.3">
-      <c r="M109" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="N109" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="O109" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="P109" s="6">
+      <c r="P102" s="5">
         <v>45408</v>
       </c>
-      <c r="Q109" s="6">
+      <c r="Q102" s="5">
         <v>45414</v>
       </c>
+      <c r="R102" s="2"/>
     </row>
     <row r="197" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D197" s="2"/>

</xml_diff>